<commit_message>
Add README.md file; Add one test to AnimalExcelParserServiceTest; Refactor project; Redesign pages
</commit_message>
<xml_diff>
--- a/src/test/resources/validAndInvalidCells.xlsx
+++ b/src/test/resources/validAndInvalidCells.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Professional\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\animalBase\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E49F60E3-3EC7-4276-A89F-1E6BC1F157A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C5DD79-5689-421C-BA9C-282FEDFD10D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{5DE14579-9BBA-4D06-BD64-A8F0B77E75CA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Тип</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>bird</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F0437AE-3CD4-4737-88F2-A60F506C8CB7}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,8 +435,8 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>45</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -451,22 +454,11 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+        <v>123.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>